<commit_message>
Add ability to export order products
</commit_message>
<xml_diff>
--- a/Mushka.Infrastructure.Excel/Templates/export_orders_template.xlsx
+++ b/Mushka.Infrastructure.Excel/Templates/export_orders_template.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MUSHKA\mushka-accounting\Mushka.Infrastructure.Excel\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Mine\MUSHKA\accounting\Mushka.Infrastructure.Excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25245" windowHeight="8685"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Orders" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
@@ -23,10 +23,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>НАИМЕНОВАНИЕ</t>
+  </si>
+  <si>
+    <t>АРТИКУЛ</t>
+  </si>
+  <si>
+    <t>РАЗМЕР</t>
+  </si>
+  <si>
+    <t>КОЛИЧЕСТВО</t>
+  </si>
+  <si>
+    <t>НА СУММУ</t>
+  </si>
+  <si>
+    <t>Заказов</t>
+  </si>
+  <si>
+    <t>Моделей</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -42,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,12 +87,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +402,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>